<commit_message>
updated creds and login scenario for Admin totara; edited API tests
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/staging/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/staging/Common_MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22568" windowHeight="9487"/>
+    <workbookView windowWidth="22568" windowHeight="9487" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -304,7 +304,7 @@
     <t>TOTARALOGINURL</t>
   </si>
   <si>
-    <t>https://totara.staging.bppdigital.buildempire.app/login/index.php</t>
+    <t>https://totara.staging.bppdigital.buildempire.app/</t>
   </si>
   <si>
     <t>CUSTOMERGROUP</t>
@@ -339,10 +339,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -389,6 +389,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -404,23 +434,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -434,6 +450,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -442,31 +481,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -480,6 +496,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -489,30 +512,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -533,187 +533,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -743,16 +743,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -766,11 +766,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -790,17 +796,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -830,27 +839,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -860,128 +860,128 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1350,8 +1350,8 @@
   <sheetPr/>
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71559633027523" defaultRowHeight="14.5" outlineLevelCol="2"/>
@@ -1756,8 +1756,8 @@
   <sheetPr/>
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
@@ -1969,7 +1969,7 @@
       <c r="A19" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="7" t="s">
         <v>95</v>
       </c>
       <c r="C19" s="10" t="s">
@@ -1990,6 +1990,7 @@
     <hyperlink ref="B8" r:id="rId9" display="https://admin.staging.bppdigital.buildempire.app"/>
     <hyperlink ref="B13" r:id="rId10" display="https://staging.bppdigital.buildempire.app/account?registration_type=jersey"/>
     <hyperlink ref="B11" r:id="rId11" display="https://staging.bppdigital.buildempire.app/account?registration_type=rbs"/>
+    <hyperlink ref="B19" r:id="rId12" display="https://totara.staging.bppdigital.buildempire.app/"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>

<commit_message>
added Digital part for PD Booking test
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/staging/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/staging/Common_MetaData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="107">
   <si>
     <t>Tag</t>
   </si>
@@ -305,6 +305,12 @@
   </si>
   <si>
     <t>https://totara.staging.bppdigital.buildempire.app/</t>
+  </si>
+  <si>
+    <t>PDCOURSEURL</t>
+  </si>
+  <si>
+    <t>https://staging.bppdigital.buildempire.app/courses/accountancy-and-tax/vat-workshop</t>
   </si>
   <si>
     <t>CUSTOMERGROUP</t>
@@ -344,7 +350,7 @@
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,8 +388,69 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -397,30 +464,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -435,64 +489,24 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -512,7 +526,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -533,103 +547,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -642,78 +728,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -743,16 +757,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -766,17 +780,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -796,20 +813,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -842,7 +856,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -860,132 +874,132 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1013,6 +1027,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="10" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="10" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1356,10 +1374,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71559633027523" defaultRowHeight="14.5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="33.8532110091743" style="14" customWidth="1"/>
-    <col min="2" max="2" width="45.4311926605505" style="14" customWidth="1"/>
-    <col min="3" max="3" width="44.1467889908257" style="14" customWidth="1"/>
-    <col min="4" max="16384" width="8.71559633027523" style="14"/>
+    <col min="1" max="1" width="33.8532110091743" style="16" customWidth="1"/>
+    <col min="2" max="2" width="45.4311926605505" style="16" customWidth="1"/>
+    <col min="3" max="3" width="44.1467889908257" style="16" customWidth="1"/>
+    <col min="4" max="16384" width="8.71559633027523" style="16"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:3">
@@ -1374,288 +1392,288 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="16" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="16" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="18" t="s">
         <v>32</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="18" t="s">
         <v>37</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="18" t="s">
         <v>47</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="18" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1704,7 +1722,7 @@
       <c r="A2" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="15" t="s">
         <v>55</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1754,10 +1772,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
@@ -1969,10 +1987,21 @@
       <c r="A19" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="13" t="s">
         <v>95</v>
       </c>
       <c r="C19" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1991,6 +2020,7 @@
     <hyperlink ref="B13" r:id="rId10" display="https://staging.bppdigital.buildempire.app/account?registration_type=jersey"/>
     <hyperlink ref="B11" r:id="rId11" display="https://staging.bppdigital.buildempire.app/account?registration_type=rbs"/>
     <hyperlink ref="B19" r:id="rId12" display="https://totara.staging.bppdigital.buildempire.app/"/>
+    <hyperlink ref="B20" r:id="rId13" display="https://staging.bppdigital.buildempire.app/courses/accountancy-and-tax/vat-workshop"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
@@ -2027,10 +2057,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -2038,10 +2068,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -2049,10 +2079,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -2060,7 +2090,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B5" s="3">
         <v>10</v>
@@ -2071,7 +2101,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B6" s="3">
         <v>2022</v>
@@ -2082,7 +2112,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B7" s="3">
         <v>737</v>

</xml_diff>

<commit_message>
changed URLS required based on BPP-10766; temporarily commented localIdentifiers in DriverProvider until BPP-11045 will be resolved
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/staging/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/staging/Common_MetaData.xlsx
@@ -235,13 +235,13 @@
     <t>BUILDEMPIREURL</t>
   </si>
   <si>
-    <t>https://staging.bppdigital.buildempire.app/account</t>
+    <t>https://web-stage-bppdigital.bppuniversity.com/account</t>
   </si>
   <si>
     <t>BUILDEMPIREADMINURL</t>
   </si>
   <si>
-    <t>https://admin.staging.bppdigital.buildempire.app</t>
+    <t>https://admin-stage-bppdigital.bppuniversity.com</t>
   </si>
   <si>
     <t>STAGINGVLENOCASLOGINURL</t>
@@ -259,7 +259,7 @@
     <t>BUILDEMPIREBESPOKEURL</t>
   </si>
   <si>
-    <t>https://staging.bppdigital.buildempire.app/account?registration_type=rbs</t>
+    <t>https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs</t>
   </si>
   <si>
     <t>BUILDEMPIRELOGINURL</t>
@@ -268,25 +268,25 @@
     <t>BUILDEMPIRECHANNELISLANDURL</t>
   </si>
   <si>
-    <t>https://staging.bppdigital.buildempire.app/account?registration_type=jersey</t>
+    <t>https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey</t>
   </si>
   <si>
     <t>BPPDIGITALINSIGHTSURL</t>
   </si>
   <si>
-    <t>https://staging.bppdigital.buildempire.app/insights</t>
+    <t>https://web-stage-bppdigital.bppuniversity.com/insights</t>
   </si>
   <si>
     <t>BPPDIGITALINDEXURL</t>
   </si>
   <si>
-    <t>https://staging.bppdigital.buildempire.app/</t>
+    <t>https://web-stage-bppdigital.bppuniversity.com</t>
   </si>
   <si>
     <t>BPPPDTESTCOURSEURL</t>
   </si>
   <si>
-    <t>https://staging.bppdigital.buildempire.app/courses/accountancy/test-automation</t>
+    <t>https://web-stage-bppdigital.bppuniversity.com/courses/accountancy/test-automation</t>
   </si>
   <si>
     <t>BPPBARCLEYCARDURL</t>
@@ -304,13 +304,13 @@
     <t>TOTARALOGINURL</t>
   </si>
   <si>
-    <t>https://totara.staging.bppdigital.buildempire.app/</t>
+    <t>https://totara-stage-bppdigital.bppuniversity.com</t>
   </si>
   <si>
     <t>PDCOURSEURL</t>
   </si>
   <si>
-    <t>https://staging.bppdigital.buildempire.app/courses/accountancy-and-tax/vat-workshop</t>
+    <t>https://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/vat-workshop</t>
   </si>
   <si>
     <t>CUSTOMERGROUP</t>
@@ -345,12 +345,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -380,6 +380,126 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -388,69 +508,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -463,76 +523,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -541,7 +533,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -559,7 +629,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -571,37 +671,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -613,7 +695,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -625,109 +707,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -756,17 +742,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -780,20 +762,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -814,6 +793,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -828,43 +831,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -874,128 +860,128 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1008,37 +994,47 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="10"/>
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="10" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="10" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1374,10 +1370,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71559633027523" defaultRowHeight="14.5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="33.8532110091743" style="16" customWidth="1"/>
-    <col min="2" max="2" width="45.4311926605505" style="16" customWidth="1"/>
-    <col min="3" max="3" width="44.1467889908257" style="16" customWidth="1"/>
-    <col min="4" max="16384" width="8.71559633027523" style="16"/>
+    <col min="1" max="1" width="33.8532110091743" style="9" customWidth="1"/>
+    <col min="2" max="2" width="45.4311926605505" style="9" customWidth="1"/>
+    <col min="3" max="3" width="44.1467889908257" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="8.71559633027523" style="9"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:3">
@@ -1392,288 +1388,288 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="12" t="s">
         <v>47</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="12" t="s">
         <v>51</v>
       </c>
       <c r="B26" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="12" t="s">
         <v>53</v>
       </c>
       <c r="B27" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="12" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1722,7 +1718,7 @@
       <c r="A2" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>55</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1775,13 +1771,13 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="52.4311926605505" customWidth="1"/>
+    <col min="2" max="2" width="52.4311926605505" style="4" customWidth="1"/>
     <col min="3" max="3" width="26.1467889908257" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1797,10 +1793,10 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1808,7 +1804,7 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>63</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -1819,7 +1815,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>65</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -1830,7 +1826,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>67</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -1841,7 +1837,7 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>69</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -1852,156 +1848,156 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2012,15 +2008,19 @@
     <hyperlink ref="B5" r:id="rId3" display="https://cod-stage.bpp.com/login/index.php"/>
     <hyperlink ref="B4" r:id="rId4" display="https://study-stage.bpp.com/login/index.php"/>
     <hyperlink ref="B3" r:id="rId5" display="https://lms-stage.bpp.com/login/index.php"/>
-    <hyperlink ref="B7" r:id="rId6" display="https://staging.bppdigital.buildempire.app/account" tooltip="https://staging.bppdigital.buildempire.app/account"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://web-stage-bppdigital.bppuniversity.com/account" tooltip="https://web-stage-bppdigital.bppuniversity.com/account"/>
     <hyperlink ref="B9" r:id="rId7" display="https://vle-stage.bppuniversity.com/vle/login/index.php?authCAS=NOCAS" tooltip="https://vle-stage.bppuniversity.com/vle/login/index.php?authCAS=NOCAS"/>
     <hyperlink ref="B10" r:id="rId8" display="http://bpp-stage.apolloglobal.int/openbravo"/>
-    <hyperlink ref="B12" r:id="rId6" display="https://staging.bppdigital.buildempire.app/account"/>
-    <hyperlink ref="B8" r:id="rId9" display="https://admin.staging.bppdigital.buildempire.app"/>
-    <hyperlink ref="B13" r:id="rId10" display="https://staging.bppdigital.buildempire.app/account?registration_type=jersey"/>
-    <hyperlink ref="B11" r:id="rId11" display="https://staging.bppdigital.buildempire.app/account?registration_type=rbs"/>
-    <hyperlink ref="B19" r:id="rId12" display="https://totara.staging.bppdigital.buildempire.app/"/>
-    <hyperlink ref="B20" r:id="rId13" display="https://staging.bppdigital.buildempire.app/courses/accountancy-and-tax/vat-workshop"/>
+    <hyperlink ref="B12" r:id="rId6" display="https://web-stage-bppdigital.bppuniversity.com/account" tooltip="https://web-stage-bppdigital.bppuniversity.com/account"/>
+    <hyperlink ref="B8" r:id="rId9" display="https://admin-stage-bppdigital.bppuniversity.com" tooltip="https://admin-stage-bppdigital.bppuniversity.com"/>
+    <hyperlink ref="B13" r:id="rId10" display="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey"/>
+    <hyperlink ref="B11" r:id="rId11" display="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs"/>
+    <hyperlink ref="B19" r:id="rId12" display="https://totara-stage-bppdigital.bppuniversity.com" tooltip="https://totara-stage-bppdigital.bppuniversity.com"/>
+    <hyperlink ref="B20" r:id="rId13" display="https://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/vat-workshop" tooltip="https://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/vat-workshop"/>
+    <hyperlink ref="B15" r:id="rId14" display="https://web-stage-bppdigital.bppuniversity.com" tooltip="https://web-stage-bppdigital.bppuniversity.com"/>
+    <hyperlink ref="B16" r:id="rId15" display="https://web-stage-bppdigital.bppuniversity.com/courses/accountancy/test-automation"/>
+    <hyperlink ref="B14" r:id="rId16" display="https://web-stage-bppdigital.bppuniversity.com/insights" tooltip="https://web-stage-bppdigital.bppuniversity.com/insights"/>
+    <hyperlink ref="B18" r:id="rId17" display="https://bppsandbox.administrateapp.com"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>

<commit_message>
updated ImageUtil Class edited PD booking test
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/staging/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/staging/Common_MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22568" windowHeight="9487" activeTab="1"/>
+    <workbookView windowWidth="22568" windowHeight="9487" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -322,7 +322,7 @@
     <t>PDCOURSEURL</t>
   </si>
   <si>
-    <t>https://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/vat-workshop</t>
+    <t>https://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1</t>
   </si>
   <si>
     <t>CUSTOMERGROUP</t>
@@ -358,9 +358,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -399,6 +399,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -406,8 +436,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -422,32 +453,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -459,44 +468,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -505,6 +476,58 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -512,29 +535,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -545,187 +545,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -754,15 +754,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -781,8 +772,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -798,32 +789,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -851,153 +816,188 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1012,13 +1012,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1027,7 +1027,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1040,13 +1040,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1061,12 +1058,12 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Currency" xfId="5" builtinId="4"/>
     <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
     <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
@@ -1444,7 +1441,7 @@
       <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -1455,7 +1452,7 @@
       <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -1477,7 +1474,7 @@
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -1499,7 +1496,7 @@
       <c r="A11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -1664,7 +1661,7 @@
       <c r="A26" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="17" t="s">
         <v>52</v>
       </c>
       <c r="C26" s="10" t="s">
@@ -1675,7 +1672,7 @@
       <c r="A27" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="18" t="s">
         <v>54</v>
       </c>
       <c r="C27" s="10" t="s">
@@ -1701,7 +1698,7 @@
   <sheetPr/>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1774,7 +1771,7 @@
       <c r="B6" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="15" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1785,7 +1782,7 @@
       <c r="B7" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1796,7 +1793,7 @@
       <c r="B8" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="15" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1812,8 +1809,8 @@
   <sheetPr/>
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
@@ -2058,7 +2055,7 @@
     <hyperlink ref="B13" r:id="rId10" display="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey"/>
     <hyperlink ref="B11" r:id="rId11" display="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs"/>
     <hyperlink ref="B19" r:id="rId12" display="https://totara-stage-bppdigital.bppuniversity.com" tooltip="https://totara-stage-bppdigital.bppuniversity.com"/>
-    <hyperlink ref="B20" r:id="rId13" display="https://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/vat-workshop" tooltip="https://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/vat-workshop"/>
+    <hyperlink ref="B20" r:id="rId13" display="https://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1" tooltip="https://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1"/>
     <hyperlink ref="B15" r:id="rId14" display="https://web-stage-bppdigital.bppuniversity.com" tooltip="https://web-stage-bppdigital.bppuniversity.com"/>
     <hyperlink ref="B16" r:id="rId15" display="https://web-stage-bppdigital.bppuniversity.com/courses/accountancy/test-automation"/>
     <hyperlink ref="B14" r:id="rId16" display="https://web-stage-bppdigital.bppuniversity.com/insights" tooltip="https://web-stage-bppdigital.bppuniversity.com/insights"/>

</xml_diff>

<commit_message>
updated PD Booking and SF Switch To Key Apps tests
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/staging/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/staging/Common_MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22568" windowHeight="9487" activeTab="1"/>
+    <workbookView windowWidth="22568" windowHeight="9487" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -322,7 +322,7 @@
     <t>PDCOURSEURL</t>
   </si>
   <si>
-    <t>https://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/vat-workshop</t>
+    <t>http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1</t>
   </si>
   <si>
     <t>CUSTOMERGROUP</t>
@@ -357,10 +357,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -400,14 +400,46 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -429,25 +461,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -459,44 +484,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -507,22 +494,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -535,6 +514,27 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -551,181 +551,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -756,9 +756,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -781,8 +798,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -802,17 +828,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -828,33 +843,21 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -866,138 +869,135 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1012,13 +1012,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1027,7 +1027,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1040,13 +1040,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1061,12 +1058,12 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Currency" xfId="5" builtinId="4"/>
     <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
     <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
@@ -1444,7 +1441,7 @@
       <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -1455,7 +1452,7 @@
       <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -1477,7 +1474,7 @@
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -1499,7 +1496,7 @@
       <c r="A11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -1664,7 +1661,7 @@
       <c r="A26" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="17" t="s">
         <v>52</v>
       </c>
       <c r="C26" s="10" t="s">
@@ -1675,7 +1672,7 @@
       <c r="A27" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="18" t="s">
         <v>54</v>
       </c>
       <c r="C27" s="10" t="s">
@@ -1701,7 +1698,7 @@
   <sheetPr/>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1774,7 +1771,7 @@
       <c r="B6" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="15" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1785,7 +1782,7 @@
       <c r="B7" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1796,7 +1793,7 @@
       <c r="B8" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="15" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1812,8 +1809,8 @@
   <sheetPr/>
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
@@ -2058,7 +2055,7 @@
     <hyperlink ref="B13" r:id="rId10" display="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey"/>
     <hyperlink ref="B11" r:id="rId11" display="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs"/>
     <hyperlink ref="B19" r:id="rId12" display="https://totara-stage-bppdigital.bppuniversity.com" tooltip="https://totara-stage-bppdigital.bppuniversity.com"/>
-    <hyperlink ref="B20" r:id="rId13" display="https://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/vat-workshop" tooltip="https://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/vat-workshop"/>
+    <hyperlink ref="B20" r:id="rId13" display="http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1" tooltip="http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1"/>
     <hyperlink ref="B15" r:id="rId14" display="https://web-stage-bppdigital.bppuniversity.com" tooltip="https://web-stage-bppdigital.bppuniversity.com"/>
     <hyperlink ref="B16" r:id="rId15" display="https://web-stage-bppdigital.bppuniversity.com/courses/accountancy/test-automation"/>
     <hyperlink ref="B14" r:id="rId16" display="https://web-stage-bppdigital.bppuniversity.com/insights" tooltip="https://web-stage-bppdigital.bppuniversity.com/insights"/>

</xml_diff>